<commit_message>
added yearly blocks data
</commit_message>
<xml_diff>
--- a/results/t-tests/ttest-results.xlsx
+++ b/results/t-tests/ttest-results.xlsx
@@ -9,6 +9,8 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="4Y Blocks" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="11Y Blocks" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="4Y Blocks Data" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="11Y Blocks Data" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -930,4 +932,415 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>1980-1983</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>1984-1987</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>1988-1991</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>1992-1995</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>1996-1999</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2000-2003</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>2004-2007</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>2008-2011</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>2012-2015</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>2016-2019</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>2020-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1984215.04</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1885275.517</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1923381.114</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1777557.862</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1862215.666</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1683637.982</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1900290.624</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1790393.904</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1815850.831</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1601410.129</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1754165.795</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1838153.82</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1940873.569</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1799819.844</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1970400.155</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1973296.457</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1783958.153</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1826529.309</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1826130.974</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1641965.98</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1700190.457</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1646240.327</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2068803.876</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1951143.692</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1942424.567</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1990792.359</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1633907.377</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1925298.682</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1842572.17</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1441530.109</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1781967.197</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1813670.267</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1513700.956</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1926352.241</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2105383.706</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2001966.894</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1790723.418</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1713535.308</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1883313.057</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1786635.778</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1763011.252</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1895202.71</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1949969.043</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1846196.197</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>1980-1990</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>1991-2001</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2002-2012</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2013-2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1984215.04</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2001966.894</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1925298.682</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1641965.98</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1838153.82</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1777557.862</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1883313.057</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1781967.197</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2068803.876</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1970400.155</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1900290.624</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1895202.71</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1926352.241</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1990792.359</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1826529.309</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1601410.129</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1885275.517</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1790723.418</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1842572.17</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1700190.457</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1940873.569</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1862215.666</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1786635.778</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1813670.267</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1951143.692</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1973296.457</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1790393.904</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1949969.043</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2105383.706</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1633907.377</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1826130.974</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1754165.795</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1923381.114</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1713535.308</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1441530.109</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1646240.327</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1799819.844</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1683637.982</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1763011.252</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1513700.956</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1942424.567</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1783958.153</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1815850.831</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1846196.197</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>